<commit_message>
Updated a little bit
</commit_message>
<xml_diff>
--- a/Example_Sites_Clearsky.xlsx
+++ b/Example_Sites_Clearsky.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11205"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\buffalo-nas\profiles$\rli\Desktop\Daily\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ray/Documents/GitHub/Clear-Sky-Model/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13395" windowHeight="8865"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26200" windowHeight="16640"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Worksheet1!$A$1:$G$87</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -372,7 +372,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0.000_);_(* \(#,##0.000\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -1267,26 +1267,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G96" sqref="G96"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="4" width="19" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" customWidth="1"/>
-    <col min="6" max="6" width="15.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" customWidth="1"/>
+    <col min="8" max="8" width="16.83203125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="11" max="11" width="16.28515625" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="11" max="11" width="16.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" ht="39" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1321,7 +1320,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="2" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -1344,7 +1343,7 @@
         <v>-118.282421</v>
       </c>
     </row>
-    <row r="3" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -1367,7 +1366,7 @@
         <v>-120.3245314</v>
       </c>
     </row>
-    <row r="4" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -1390,7 +1389,7 @@
         <v>-118.29639299999999</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
@@ -1426,7 +1425,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -1449,7 +1448,7 @@
         <v>-81.333720999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>17</v>
       </c>
@@ -1472,7 +1471,7 @@
         <v>-118.306</v>
       </c>
     </row>
-    <row r="8" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>-118.307</v>
       </c>
     </row>
-    <row r="9" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>19</v>
       </c>
@@ -1518,7 +1517,7 @@
         <v>-118.324</v>
       </c>
     </row>
-    <row r="10" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>-118.02447100000001</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>21</v>
       </c>
@@ -1577,7 +1576,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -1600,7 +1599,7 @@
         <v>-118.023684</v>
       </c>
     </row>
-    <row r="13" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>23</v>
       </c>
@@ -1623,7 +1622,7 @@
         <v>-77.780794</v>
       </c>
     </row>
-    <row r="14" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1646,7 +1645,7 @@
         <v>-79.771799999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>25</v>
       </c>
@@ -1669,7 +1668,7 @@
         <v>-118.233</v>
       </c>
     </row>
-    <row r="16" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
@@ -1692,7 +1691,7 @@
         <v>-120.43043400000001</v>
       </c>
     </row>
-    <row r="17" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>-118.280901</v>
       </c>
     </row>
-    <row r="18" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>28</v>
       </c>
@@ -1730,7 +1729,7 @@
         <v>-118.311824</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>29</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="20" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>31</v>
       </c>
@@ -1784,7 +1783,7 @@
         <v>-118.303039</v>
       </c>
     </row>
-    <row r="21" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>30</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>-79.730037999999993</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="28" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>32</v>
       </c>
@@ -1842,7 +1841,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>33</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>-117.3429891</v>
       </c>
     </row>
-    <row r="24" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>34</v>
       </c>
@@ -1888,7 +1887,7 @@
         <v>-117.3421659</v>
       </c>
     </row>
-    <row r="25" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>35</v>
       </c>
@@ -1911,7 +1910,7 @@
         <v>-79.127650000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>36</v>
       </c>
@@ -1934,7 +1933,7 @@
         <v>-118.81600299999999</v>
       </c>
     </row>
-    <row r="27" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>37</v>
       </c>
@@ -1957,7 +1956,7 @@
         <v>-87.308224999999993</v>
       </c>
     </row>
-    <row r="28" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>-117.45679199999999</v>
       </c>
     </row>
-    <row r="29" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>41</v>
       </c>
@@ -2003,7 +2002,7 @@
         <v>-82.357406999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>42</v>
       </c>
@@ -2026,7 +2025,7 @@
         <v>-81.764240000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>43</v>
       </c>
@@ -2049,7 +2048,7 @@
         <v>-78.94</v>
       </c>
     </row>
-    <row r="32" spans="1:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>44</v>
       </c>
@@ -2072,7 +2071,7 @@
         <v>-78.040000000000006</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>45</v>
       </c>
@@ -2095,7 +2094,7 @@
         <v>-87.453192000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>46</v>
       </c>
@@ -2118,7 +2117,7 @@
         <v>-118.2918712</v>
       </c>
     </row>
-    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>47</v>
       </c>
@@ -2141,7 +2140,7 @@
         <v>-72.891000000000005</v>
       </c>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>49</v>
       </c>
@@ -2164,7 +2163,7 @@
         <v>-117.93887599999999</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>50</v>
       </c>
@@ -2187,7 +2186,7 @@
         <v>-118.278638</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>51</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>-117.192798</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>52</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>-79.545501000000002</v>
       </c>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>53</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>-72.092990549999996</v>
       </c>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
         <v>55</v>
       </c>
@@ -2275,7 +2274,7 @@
         <v>-118.31316700000001</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>56</v>
       </c>
@@ -2298,7 +2297,7 @@
         <v>-117.192778</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>58</v>
       </c>
@@ -2321,7 +2320,7 @@
         <v>-117.9396539</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>59</v>
       </c>
@@ -2344,7 +2343,7 @@
         <v>-117.1436947</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>60</v>
       </c>
@@ -2367,7 +2366,7 @@
         <v>-118.812617</v>
       </c>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>61</v>
       </c>
@@ -2390,7 +2389,7 @@
         <v>-118.2905717</v>
       </c>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>62</v>
       </c>
@@ -2413,7 +2412,7 @@
         <v>-118.2915991</v>
       </c>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>63</v>
       </c>
@@ -2436,7 +2435,7 @@
         <v>-111.45192969999999</v>
       </c>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>65</v>
       </c>
@@ -2459,7 +2458,7 @@
         <v>-78.180682000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>66</v>
       </c>
@@ -2482,7 +2481,7 @@
         <v>-117.9396539</v>
       </c>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>67</v>
       </c>
@@ -2505,7 +2504,7 @@
         <v>-118.3376205</v>
       </c>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>68</v>
       </c>
@@ -2528,7 +2527,7 @@
         <v>-118.297884</v>
       </c>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>69</v>
       </c>
@@ -2551,7 +2550,7 @@
         <v>-72.098988259999999</v>
       </c>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>70</v>
       </c>
@@ -2574,7 +2573,7 @@
         <v>-72.011099999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>71</v>
       </c>
@@ -2597,7 +2596,7 @@
         <v>-72.011099999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>72</v>
       </c>
@@ -2620,7 +2619,7 @@
         <v>-72.011099999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>73</v>
       </c>
@@ -2643,7 +2642,7 @@
         <v>-72.011099999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>74</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>-72.180568480000005</v>
       </c>
     </row>
-    <row r="59" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>75</v>
       </c>
@@ -2689,7 +2688,7 @@
         <v>-72.180568480000005</v>
       </c>
     </row>
-    <row r="60" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>76</v>
       </c>
@@ -2712,7 +2711,7 @@
         <v>-72.180568480000005</v>
       </c>
     </row>
-    <row r="61" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>77</v>
       </c>
@@ -2735,7 +2734,7 @@
         <v>-72.180568480000005</v>
       </c>
     </row>
-    <row r="62" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>78</v>
       </c>
@@ -2758,7 +2757,7 @@
         <v>-72.743595940000006</v>
       </c>
     </row>
-    <row r="63" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>79</v>
       </c>
@@ -2781,7 +2780,7 @@
         <v>-118.309</v>
       </c>
     </row>
-    <row r="64" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>80</v>
       </c>
@@ -2804,7 +2803,7 @@
         <v>-118.29131889999999</v>
       </c>
     </row>
-    <row r="65" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>81</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>-118.2912171</v>
       </c>
     </row>
-    <row r="66" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>82</v>
       </c>
@@ -2850,7 +2849,7 @@
         <v>-118.2938302</v>
       </c>
     </row>
-    <row r="67" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>83</v>
       </c>
@@ -2873,7 +2872,7 @@
         <v>-118.2939958</v>
       </c>
     </row>
-    <row r="68" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>84</v>
       </c>
@@ -2896,7 +2895,7 @@
         <v>-72.743420670000006</v>
       </c>
     </row>
-    <row r="69" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>85</v>
       </c>
@@ -2919,7 +2918,7 @@
         <v>-78.971999999999994</v>
       </c>
     </row>
-    <row r="70" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>86</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>-79.104374000000007</v>
       </c>
     </row>
-    <row r="71" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>87</v>
       </c>
@@ -2965,7 +2964,7 @@
         <v>-87.159819999999996</v>
       </c>
     </row>
-    <row r="72" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>88</v>
       </c>
@@ -2988,7 +2987,7 @@
         <v>-117.4722154</v>
       </c>
     </row>
-    <row r="73" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
         <v>90</v>
       </c>
@@ -3011,7 +3010,7 @@
         <v>-117.4702734</v>
       </c>
     </row>
-    <row r="74" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>91</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>-117.3872812</v>
       </c>
     </row>
-    <row r="75" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
         <v>92</v>
       </c>
@@ -3057,7 +3056,7 @@
         <v>-117.38730099999999</v>
       </c>
     </row>
-    <row r="76" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
         <v>93</v>
       </c>
@@ -3080,7 +3079,7 @@
         <v>-117.3872325</v>
       </c>
     </row>
-    <row r="77" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>94</v>
       </c>
@@ -3103,7 +3102,7 @@
         <v>-117.3875555</v>
       </c>
     </row>
-    <row r="78" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
         <v>95</v>
       </c>
@@ -3126,7 +3125,7 @@
         <v>-118.3197687</v>
       </c>
     </row>
-    <row r="79" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>96</v>
       </c>
@@ -3145,7 +3144,7 @@
         <v>-118.3197687</v>
       </c>
     </row>
-    <row r="80" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
         <v>97</v>
       </c>
@@ -3168,7 +3167,7 @@
         <v>-118.191244</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>98</v>
       </c>
@@ -3187,7 +3186,7 @@
         <v>-118.31350500000001</v>
       </c>
     </row>
-    <row r="82" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>99</v>
       </c>
@@ -3210,7 +3209,7 @@
         <v>-78.022685769999995</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>100</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>-78.100949999999997</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>101</v>
       </c>
@@ -3256,7 +3255,7 @@
         <v>-78.052019000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
         <v>102</v>
       </c>
@@ -3279,7 +3278,7 @@
         <v>-85.042861000000002</v>
       </c>
     </row>
-    <row r="86" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>103</v>
       </c>
@@ -3302,7 +3301,7 @@
         <v>-71.936541120000001</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
         <v>104</v>
       </c>
@@ -3326,16 +3325,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G87">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Aspiration G"/>
-        <filter val="Beacon 3"/>
-        <filter val="Eden"/>
-        <filter val="Expressway A"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:G87"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>